<commit_message>
Added fix in the computation
</commit_message>
<xml_diff>
--- a/distillery/tests/TestCase/TestCase.xlsx
+++ b/distillery/tests/TestCase/TestCase.xlsx
@@ -9,18 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7872" firstSheet="7" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7872" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="TestCase01" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet15" sheetId="15" r:id="rId2"/>
-    <sheet name="TestCase02" sheetId="2" r:id="rId3"/>
-    <sheet name="TestCase03" sheetId="3" r:id="rId4"/>
-    <sheet name="TestCase04" sheetId="4" r:id="rId5"/>
-    <sheet name="TestCase05" sheetId="5" r:id="rId6"/>
-    <sheet name="TestCase06" sheetId="6" r:id="rId7"/>
-    <sheet name="TestCase07" sheetId="7" r:id="rId8"/>
-    <sheet name="TestCase08" sheetId="8" r:id="rId9"/>
+    <sheet name="TestCase02" sheetId="2" r:id="rId2"/>
+    <sheet name="TestCase03" sheetId="3" r:id="rId3"/>
+    <sheet name="TestCase04" sheetId="4" r:id="rId4"/>
+    <sheet name="TestCase05" sheetId="5" r:id="rId5"/>
+    <sheet name="TestCase06" sheetId="6" r:id="rId6"/>
+    <sheet name="TestCase07" sheetId="7" r:id="rId7"/>
+    <sheet name="TestCase08" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet15" sheetId="15" r:id="rId9"/>
     <sheet name="TestCase09" sheetId="9" r:id="rId10"/>
     <sheet name="TestCase10" sheetId="10" r:id="rId11"/>
     <sheet name="TestCase11" sheetId="11" r:id="rId12"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="37">
   <si>
     <t>Distillery</t>
   </si>
@@ -104,13 +104,58 @@
   </si>
   <si>
     <t>Newly added pitch</t>
+  </si>
+  <si>
+    <t>MANDAUE</t>
+  </si>
+  <si>
+    <t>BARREL</t>
+  </si>
+  <si>
+    <t>KKK</t>
+  </si>
+  <si>
+    <t>diff</t>
+  </si>
+  <si>
+    <t>age(younger)</t>
+  </si>
+  <si>
+    <t>age(older)</t>
+  </si>
+  <si>
+    <t>HAPPY</t>
+  </si>
+  <si>
+    <t>CARLA</t>
+  </si>
+  <si>
+    <t>LILY</t>
+  </si>
+  <si>
+    <t>BBB</t>
+  </si>
+  <si>
+    <t>CCC</t>
+  </si>
+  <si>
+    <t>OCTA</t>
+  </si>
+  <si>
+    <t>AAA</t>
+  </si>
+  <si>
+    <t>HEXA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OCTA </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,6 +167,19 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -147,10 +205,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,7 +495,7 @@
   <dimension ref="B2:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -644,8 +705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -661,18 +722,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E10"/>
   <sheetViews>
@@ -774,81 +823,1001 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F10"/>
+  <dimension ref="B2:J23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D23" sqref="D23:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="16.77734375" customWidth="1"/>
+    <col min="6" max="8" width="9.109375" customWidth="1"/>
+    <col min="9" max="9" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="D4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="2">
         <v>43968</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
         <v>2</v>
       </c>
       <c r="E5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F5">
+        <f>1.19-1.02</f>
+        <v>0.16999999999999993</v>
+      </c>
+      <c r="G5">
+        <f>2019+2019</f>
+        <v>4038</v>
+      </c>
+      <c r="H5">
+        <f>2018+2018</f>
+        <v>4036</v>
+      </c>
+      <c r="I5">
+        <f>(F5)/(G5-H5)</f>
+        <v>8.4999999999999964E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <f>1.19-1.01</f>
+        <v>0.17999999999999994</v>
+      </c>
+      <c r="G6">
+        <f>2019+2019.25</f>
+        <v>4038.25</v>
+      </c>
+      <c r="H6">
+        <f>2018+2018</f>
+        <v>4036</v>
+      </c>
+      <c r="I6">
+        <f>(F6)/(G6-H6)</f>
+        <v>7.9999999999999974E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F7">
+        <f>1.19-1.01</f>
+        <v>0.17999999999999994</v>
+      </c>
+      <c r="G7">
+        <f>2019+2019.25</f>
+        <v>4038.25</v>
+      </c>
+      <c r="H7">
+        <f>2019+2019</f>
+        <v>4038</v>
+      </c>
+      <c r="I7">
+        <f>(F7)/(G7-H7)</f>
+        <v>0.71999999999999975</v>
+      </c>
+      <c r="J7">
+        <f>SUM(I5:I7)/3</f>
+        <v>0.29499999999999987</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="D8" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F8">
+        <f>1.2-1.08</f>
+        <v>0.11999999999999988</v>
+      </c>
+      <c r="G8">
+        <f>2018+2018.25</f>
+        <v>4036.25</v>
+      </c>
+      <c r="H8">
+        <f>2017+2017</f>
+        <v>4034</v>
+      </c>
+      <c r="I8">
+        <f>(F8)/(G8-H8)</f>
+        <v>5.3333333333333281E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="D9" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <f>1.2-1.01</f>
+        <v>0.18999999999999995</v>
+      </c>
+      <c r="G9">
+        <f>2018+2018.5</f>
+        <v>4036.5</v>
+      </c>
+      <c r="H9">
+        <f>2017+2017</f>
+        <v>4034</v>
+      </c>
+      <c r="I9">
+        <f>(F9)/(G9-H9)</f>
+        <v>7.5999999999999984E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E10" t="s">
         <v>4</v>
+      </c>
+      <c r="F10">
+        <f>1.2-1.04</f>
+        <v>0.15999999999999992</v>
+      </c>
+      <c r="G10">
+        <f>2018+2018.5</f>
+        <v>4036.5</v>
+      </c>
+      <c r="H10">
+        <f>2018+2018.25</f>
+        <v>4036.25</v>
+      </c>
+      <c r="I10">
+        <f>(F10)/(G10-H10)</f>
+        <v>0.63999999999999968</v>
+      </c>
+      <c r="J10">
+        <f>SUM(I8:I10)/3</f>
+        <v>0.25644444444444431</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <f>1.6-1.01</f>
+        <v>0.59000000000000008</v>
+      </c>
+      <c r="G11">
+        <f>2018+2018.5</f>
+        <v>4036.5</v>
+      </c>
+      <c r="H11">
+        <f>2018+2018.25</f>
+        <v>4036.25</v>
+      </c>
+      <c r="I11">
+        <f>(F11)/(G11-H11)</f>
+        <v>2.3600000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12">
+        <f>1.6-1.02</f>
+        <v>0.58000000000000007</v>
+      </c>
+      <c r="G12">
+        <f>2019+2019.5</f>
+        <v>4038.5</v>
+      </c>
+      <c r="H12">
+        <f>2018+2018.25</f>
+        <v>4036.25</v>
+      </c>
+      <c r="I12">
+        <f>(F12)/(G12-H12)</f>
+        <v>0.25777777777777783</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13">
+        <f>1.9-1.02</f>
+        <v>0.87999999999999989</v>
+      </c>
+      <c r="G13">
+        <f>2019+2019.25</f>
+        <v>4038.25</v>
+      </c>
+      <c r="H13">
+        <f>2018+2018.5</f>
+        <v>4036.5</v>
+      </c>
+      <c r="I13">
+        <f>(F13)/(G13-H13)</f>
+        <v>0.50285714285714278</v>
+      </c>
+      <c r="J13">
+        <f>SUM(I11:I13)/3</f>
+        <v>1.0402116402116401</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14">
+        <f>1.9-1</f>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="G14">
+        <f>2016.75+2016.5</f>
+        <v>4033.25</v>
+      </c>
+      <c r="H14">
+        <f>2016+2016.5</f>
+        <v>4032.5</v>
+      </c>
+      <c r="I14">
+        <f>(F14)/(G14-H14)</f>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15">
+        <f>1.9-1.02</f>
+        <v>0.87999999999999989</v>
+      </c>
+      <c r="G15">
+        <f>2017+2017.25</f>
+        <v>4034.25</v>
+      </c>
+      <c r="H15">
+        <f>2016+2016.5</f>
+        <v>4032.5</v>
+      </c>
+      <c r="I15">
+        <f t="shared" ref="I15:I23" si="0">(F15)/(G15-H15)</f>
+        <v>0.50285714285714278</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16">
+        <f>1.9-1.02</f>
+        <v>0.87999999999999989</v>
+      </c>
+      <c r="G16">
+        <f>2017+2017.25</f>
+        <v>4034.25</v>
+      </c>
+      <c r="H16">
+        <f>2016+2016.75</f>
+        <v>4032.75</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>0.58666666666666656</v>
+      </c>
+      <c r="J16">
+        <f>SUM(I14:I16)/3</f>
+        <v>0.76317460317460306</v>
+      </c>
+    </row>
+    <row r="17" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17">
+        <f>1.19-1.03</f>
+        <v>0.15999999999999992</v>
+      </c>
+      <c r="G17">
+        <f>2018+2018.5</f>
+        <v>4036.5</v>
+      </c>
+      <c r="H17">
+        <f>2018+2018</f>
+        <v>4036</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>0.31999999999999984</v>
+      </c>
+    </row>
+    <row r="18" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18">
+        <f>1.19-1.04</f>
+        <v>0.14999999999999991</v>
+      </c>
+      <c r="G18">
+        <f>2019+2019.5</f>
+        <v>4038.5</v>
+      </c>
+      <c r="H18">
+        <f>2018+2018</f>
+        <v>4036</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999963E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19">
+        <f>1.7-1.04</f>
+        <v>0.65999999999999992</v>
+      </c>
+      <c r="G19">
+        <f>2019+2019.5</f>
+        <v>4038.5</v>
+      </c>
+      <c r="H19">
+        <f>2018+2018.5</f>
+        <v>4036.5</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="0"/>
+        <v>0.32999999999999996</v>
+      </c>
+      <c r="J19">
+        <f>SUM(I17:I19)/3</f>
+        <v>0.23666666666666658</v>
+      </c>
+    </row>
+    <row r="20" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D20" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20">
+        <f>1.9-1.04</f>
+        <v>0.85999999999999988</v>
+      </c>
+      <c r="G20">
+        <f>2019+2019.5</f>
+        <v>4038.5</v>
+      </c>
+      <c r="H20">
+        <f>2019+2019.25</f>
+        <v>4038.25</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="0"/>
+        <v>3.4399999999999995</v>
+      </c>
+    </row>
+    <row r="21" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21">
+        <f>1.9-1.02</f>
+        <v>0.87999999999999989</v>
+      </c>
+      <c r="G21">
+        <f>2019+2019.75</f>
+        <v>4038.75</v>
+      </c>
+      <c r="H21">
+        <f>2019+2019.25</f>
+        <v>4038.25</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="0"/>
+        <v>1.7599999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D22" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22">
+        <f>1.17-1.02</f>
+        <v>0.14999999999999991</v>
+      </c>
+      <c r="G22">
+        <f>2019+2019.75</f>
+        <v>4038.75</v>
+      </c>
+      <c r="H22">
+        <f>2019+2019.5</f>
+        <v>4038.5</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="0"/>
+        <v>0.59999999999999964</v>
+      </c>
+      <c r="J22">
+        <f>SUM(I20:I22)/3</f>
+        <v>1.9333333333333329</v>
+      </c>
+    </row>
+    <row r="23" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D23" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:J22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4:H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="14.21875" customWidth="1"/>
+    <col min="9" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="3">
+        <v>43968</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <f>1.15-1.04</f>
+        <v>0.10999999999999988</v>
+      </c>
+      <c r="G5">
+        <f>2018+2018.25</f>
+        <v>4036.25</v>
+      </c>
+      <c r="H5">
+        <f>2018+2018</f>
+        <v>4036</v>
+      </c>
+      <c r="I5">
+        <f>F5/(G5-H5)</f>
+        <v>0.4399999999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <f>1.15-1.06</f>
+        <v>8.9999999999999858E-2</v>
+      </c>
+      <c r="G6">
+        <f>2019+2019.75</f>
+        <v>4038.75</v>
+      </c>
+      <c r="H6">
+        <f>2018+2018</f>
+        <v>4036</v>
+      </c>
+      <c r="I6">
+        <f t="shared" ref="I6:I22" si="0">F6/(G6-H6)</f>
+        <v>3.2727272727272674E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <f>1.5-1.06</f>
+        <v>0.43999999999999995</v>
+      </c>
+      <c r="G7">
+        <f>2019+2019.75</f>
+        <v>4038.75</v>
+      </c>
+      <c r="H7">
+        <f>2018+2018.25</f>
+        <v>4036.25</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="J7">
+        <f>SUM(I5:I7)/3</f>
+        <v>0.21624242424242404</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8">
+        <f>2.7-1.12</f>
+        <v>1.58</v>
+      </c>
+      <c r="G8">
+        <f>2018+2018.5</f>
+        <v>4036.5</v>
+      </c>
+      <c r="H8">
+        <f>2018+2018.25</f>
+        <v>4036.25</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>6.32</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9">
+        <f>2.7-1.15</f>
+        <v>1.5500000000000003</v>
+      </c>
+      <c r="G9">
+        <f>2019+2019.25</f>
+        <v>4038.25</v>
+      </c>
+      <c r="H9">
+        <f>2018+2018.25</f>
+        <v>4036.25</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>0.77500000000000013</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10">
+        <f>1.6-1.15</f>
+        <v>0.45000000000000018</v>
+      </c>
+      <c r="G10">
+        <f>2019+2019.25</f>
+        <v>4038.25</v>
+      </c>
+      <c r="H10">
+        <f>2018+2018.5</f>
+        <v>4036.5</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>0.25714285714285723</v>
+      </c>
+      <c r="J10">
+        <f>SUM(I8:I10)/3</f>
+        <v>2.4507142857142861</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11">
+        <f>1.5-1.1</f>
+        <v>0.39999999999999991</v>
+      </c>
+      <c r="G11">
+        <f>2017+2017.25</f>
+        <v>4034.25</v>
+      </c>
+      <c r="H11">
+        <f>2016+2016.25</f>
+        <v>4032.25</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>0.19999999999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12">
+        <f>1.5-0.95</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G12">
+        <f>2018+2018.25</f>
+        <v>4036.25</v>
+      </c>
+      <c r="H12">
+        <f>2016+2016.25</f>
+        <v>4032.25</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>0.13750000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13">
+        <f>1.16-0.95</f>
+        <v>0.20999999999999996</v>
+      </c>
+      <c r="G13">
+        <f>2018+2018.25</f>
+        <v>4036.25</v>
+      </c>
+      <c r="H13">
+        <f>2017+2017.25</f>
+        <v>4034.25</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>0.10499999999999998</v>
+      </c>
+      <c r="J13">
+        <f>SUM(I11:I13)/3</f>
+        <v>0.14749999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14">
+        <f>1.29-1.05</f>
+        <v>0.24</v>
+      </c>
+      <c r="G14">
+        <f>2019+2019</f>
+        <v>4038</v>
+      </c>
+      <c r="H14">
+        <f>2018+2018.75</f>
+        <v>4036.75</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>0.192</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15">
+        <f>1.29-0.95</f>
+        <v>0.34000000000000008</v>
+      </c>
+      <c r="G15">
+        <f>2019+2019.25</f>
+        <v>4038.25</v>
+      </c>
+      <c r="H15">
+        <f>2018+2018.75</f>
+        <v>4036.75</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>0.22666666666666671</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16">
+        <f>1.35-0.95</f>
+        <v>0.40000000000000013</v>
+      </c>
+      <c r="G16">
+        <f>2019+2019.25</f>
+        <v>4038.25</v>
+      </c>
+      <c r="H16">
+        <f>2019+2019</f>
+        <v>4038</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>1.6000000000000005</v>
+      </c>
+      <c r="J16">
+        <f>SUM(I14:I16)/3</f>
+        <v>0.67288888888888909</v>
+      </c>
+    </row>
+    <row r="17" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17">
+        <f>1.27-0.99</f>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G17">
+        <f>2018+2018</f>
+        <v>4036</v>
+      </c>
+      <c r="H17">
+        <f>2017+2017.25</f>
+        <v>4034.25</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="18" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18">
+        <f>1.27-0.95</f>
+        <v>0.32000000000000006</v>
+      </c>
+      <c r="G18">
+        <f>2018+2018.5</f>
+        <v>4036.5</v>
+      </c>
+      <c r="H18">
+        <f>2017+2017.25</f>
+        <v>4034.25</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="0"/>
+        <v>0.14222222222222225</v>
+      </c>
+    </row>
+    <row r="19" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19">
+        <f>1.18-0.95</f>
+        <v>0.22999999999999998</v>
+      </c>
+      <c r="G19">
+        <f>2018+2018.5</f>
+        <v>4036.5</v>
+      </c>
+      <c r="H19">
+        <f>2018+2018</f>
+        <v>4036</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="0"/>
+        <v>0.45999999999999996</v>
+      </c>
+      <c r="J19">
+        <f>SUM(I17:I19)/3</f>
+        <v>0.25407407407407406</v>
+      </c>
+    </row>
+    <row r="20" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D20" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20">
+        <f>1.3</f>
+        <v>1.3</v>
+      </c>
+      <c r="G20">
+        <f>2018+2018.5</f>
+        <v>4036.5</v>
+      </c>
+      <c r="H20">
+        <f>2018+2018.25</f>
+        <v>4036.25</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="0"/>
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="21" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D21" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21">
+        <f>1.3-0.95</f>
+        <v>0.35000000000000009</v>
+      </c>
+      <c r="G21">
+        <f>2018+2018.75</f>
+        <v>4036.75</v>
+      </c>
+      <c r="H21">
+        <f>2018+2018.25</f>
+        <v>4036.25</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="0"/>
+        <v>0.70000000000000018</v>
+      </c>
+    </row>
+    <row r="22" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22">
+        <f>1.3-0.95</f>
+        <v>0.35000000000000009</v>
+      </c>
+      <c r="G22">
+        <f>2018+2018.75</f>
+        <v>4036.75</v>
+      </c>
+      <c r="H22">
+        <f>2018+2018.5</f>
+        <v>4036.5</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="0"/>
+        <v>1.4000000000000004</v>
+      </c>
+      <c r="J22">
+        <f>SUM(I20:I22)/3</f>
+        <v>2.4333333333333336</v>
       </c>
     </row>
   </sheetData>
@@ -858,80 +1827,344 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F10"/>
+  <dimension ref="B3:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D5" sqref="D5:J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="14.21875" customWidth="1"/>
-    <col min="6" max="6" width="12.21875" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D4" s="1" t="s">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="2">
         <v>43968</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6">
+        <f>0-1.02</f>
+        <v>-1.02</v>
+      </c>
+      <c r="G6">
+        <f>2019+2019.25</f>
+        <v>4038.25</v>
+      </c>
+      <c r="H6">
+        <f>2019+2019</f>
+        <v>4038</v>
+      </c>
+      <c r="I6">
+        <f>F6/(G6-H6)</f>
+        <v>-4.08</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7">
+        <f>0-1</f>
+        <v>-1</v>
+      </c>
+      <c r="G7">
+        <f>2019+2019.5</f>
+        <v>4038.5</v>
+      </c>
+      <c r="H7">
+        <f>2019+2019</f>
+        <v>4038</v>
+      </c>
+      <c r="I7">
+        <f t="shared" ref="I7:I17" si="0">F7/(G7-H7)</f>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="D8" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="E8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+      <c r="F8">
+        <f>1.19-1</f>
+        <v>0.18999999999999995</v>
+      </c>
+      <c r="G8">
+        <f>2019+2019.5</f>
+        <v>4038.5</v>
+      </c>
+      <c r="H8">
+        <f>2019+2019.25</f>
+        <v>4038.25</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>0.75999999999999979</v>
+      </c>
+      <c r="J8">
+        <f>SUM(I6:I8)/3</f>
+        <v>-1.7733333333333334</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="D9" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="E9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+      <c r="F9">
+        <f>1.2-1.03</f>
+        <v>0.16999999999999993</v>
+      </c>
+      <c r="G9">
+        <f>2018+2018.75</f>
+        <v>4036.75</v>
+      </c>
+      <c r="H9">
+        <f>2018+2018.5</f>
+        <v>4036.5</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>0.67999999999999972</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="E10" t="s">
-        <v>4</v>
+        <v>34</v>
+      </c>
+      <c r="F10">
+        <f>1.2-1.04</f>
+        <v>0.15999999999999992</v>
+      </c>
+      <c r="G10">
+        <f>2019+2019.25</f>
+        <v>4038.25</v>
+      </c>
+      <c r="H10">
+        <f>2018+2018.5</f>
+        <v>4036.5</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>9.1428571428571387E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11">
+        <f>1.19-1.04</f>
+        <v>0.14999999999999991</v>
+      </c>
+      <c r="G11">
+        <f>2019+2019.25</f>
+        <v>4038.25</v>
+      </c>
+      <c r="H11">
+        <f>2018+2018.75</f>
+        <v>4036.75</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>9.9999999999999936E-2</v>
+      </c>
+      <c r="J11">
+        <f>SUM(I9:I11)/3</f>
+        <v>0.29047619047619039</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12">
+        <f>1.21-1.04</f>
+        <v>0.16999999999999993</v>
+      </c>
+      <c r="G12">
+        <f>2019+2019.25</f>
+        <v>4038.25</v>
+      </c>
+      <c r="H12">
+        <f>2019+2019</f>
+        <v>4038</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>0.67999999999999972</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13">
+        <f>1.21-1.02</f>
+        <v>0.18999999999999995</v>
+      </c>
+      <c r="G13">
+        <f>2019+2019.5</f>
+        <v>4038.5</v>
+      </c>
+      <c r="H13">
+        <f>2019+2019</f>
+        <v>4038</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>0.37999999999999989</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14">
+        <f>1.25-1.02</f>
+        <v>0.22999999999999998</v>
+      </c>
+      <c r="G14">
+        <f>2019+2019.5</f>
+        <v>4038.5</v>
+      </c>
+      <c r="H14">
+        <f>2019+2019.25</f>
+        <v>4038.25</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>0.91999999999999993</v>
+      </c>
+      <c r="J14">
+        <f>SUM(I12:I14)/3</f>
+        <v>0.65999999999999981</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15">
+        <f>1.19-1.02</f>
+        <v>0.16999999999999993</v>
+      </c>
+      <c r="G15">
+        <f>2019+2019.25</f>
+        <v>4038.25</v>
+      </c>
+      <c r="H15">
+        <f>2018+2018</f>
+        <v>4036</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>7.5555555555555529E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16">
+        <f>1.19-1.02</f>
+        <v>0.16999999999999993</v>
+      </c>
+      <c r="G16">
+        <f>2019+2019.75</f>
+        <v>4038.75</v>
+      </c>
+      <c r="H16">
+        <f>2018+2018</f>
+        <v>4036</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>6.1818181818181793E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17">
+        <f>1.19-1.02</f>
+        <v>0.16999999999999993</v>
+      </c>
+      <c r="G17">
+        <f>2019+2019.75</f>
+        <v>4038.75</v>
+      </c>
+      <c r="H17">
+        <f>2019+2019.25</f>
+        <v>4038.25</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>0.33999999999999986</v>
+      </c>
+      <c r="J17">
+        <f>SUM(I15:I17)/3</f>
+        <v>0.15912457912457906</v>
       </c>
     </row>
   </sheetData>
@@ -941,79 +2174,153 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:F11"/>
+  <dimension ref="B3:J17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="D5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="2">
         <v>43968</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="D8" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="E8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+      <c r="J8">
+        <f>SUM(I6:I8)/3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="D9" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="E9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="E10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="E11" t="s">
-        <v>4</v>
+        <v>34</v>
+      </c>
+      <c r="J11">
+        <f>SUM(I9:I11)/3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" t="s">
+        <v>31</v>
+      </c>
+      <c r="J14">
+        <f>SUM(I12:I14)/3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" t="s">
+        <v>31</v>
+      </c>
+      <c r="J17">
+        <f>SUM(I15:I17)/3</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1022,88 +2329,6 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:F11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:F11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="6" max="6" width="16.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" s="2">
-        <v>43968</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="D11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F10"/>
   <sheetViews>
@@ -1187,7 +2412,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2"/>
   <sheetViews>
@@ -1205,4 +2430,35 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="H6:I7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="6" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="8:9" x14ac:dyDescent="0.3">
+      <c r="H7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added fixes for computation
</commit_message>
<xml_diff>
--- a/distillery/tests/TestCase/TestCase.xlsx
+++ b/distillery/tests/TestCase/TestCase.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Practice\git_repository\distillery\AnnualReturnCalculator\distillery\tests\TestCase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Distillery\tests\TestCase\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7872" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7872" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="TestCase01" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="37">
   <si>
     <t>Distillery</t>
   </si>
@@ -120,7 +120,13 @@
     <t>Refer to testData test_case_03.txt</t>
   </si>
   <si>
+    <t xml:space="preserve">  *  2019, Q3 is not included in computation</t>
+  </si>
+  <si>
     <t xml:space="preserve">  *  2018, Q3 is not included in computation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  *  2018, Q2 is not included in computation</t>
   </si>
   <si>
     <t>Younger pitch buy price is higher than older pitch sellPrice</t>
@@ -944,8 +950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1044,7 +1050,7 @@
         <v>0.42</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="4:5" x14ac:dyDescent="0.3">
@@ -1062,7 +1068,7 @@
   <dimension ref="B3:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D5" sqref="D5:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1144,7 +1150,12 @@
       <c r="F10">
         <v>0.52</v>
       </c>
-      <c r="H10" s="4"/>
+      <c r="G10">
+        <v>0.68</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
@@ -1157,9 +1168,11 @@
         <v>0.37330000000000002</v>
       </c>
       <c r="G11">
-        <v>0.32499999999999901</v>
-      </c>
-      <c r="H11" s="4"/>
+        <v>0.23</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1184,7 +1197,7 @@
   <sheetData>
     <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
@@ -1272,7 +1285,7 @@
         <v>-5.1666666666666701E-2</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1377,12 +1390,12 @@
         <v>0.42</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C14" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1394,7 +1407,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
@@ -1407,17 +1420,17 @@
     </row>
     <row r="5" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D8" s="6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>